<commit_message>
AC Sweep analyze finilized
</commit_message>
<xml_diff>
--- a/OOP2025_Project_ScoresAllocation (2).xlsx
+++ b/OOP2025_Project_ScoresAllocation (2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erfan\Dev\Cpp\sutSpice_phase2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED87E76-310E-414B-8F8F-05ADD099B4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E60088D-729F-4A70-ACBD-5BD9E567B93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>عنوان</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
@@ -511,6 +514,174 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -518,33 +689,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="6" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -567,147 +711,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -936,8 +939,8 @@
   </sheetPr>
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A34" zoomScale="97" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A32" zoomScale="118" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -948,83 +951,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="40"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="57"/>
       <c r="J2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="42"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="2">
         <v>5</v>
       </c>
-      <c r="K3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
       <c r="J4" s="2"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="65"/>
       <c r="J5" s="2">
         <v>15</v>
       </c>
@@ -1033,34 +1038,36 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A6" s="55"/>
-      <c r="B6" s="48" t="s">
+      <c r="A6" s="67"/>
+      <c r="B6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="50"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="42"/>
       <c r="J6" s="11">
         <v>18</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="K6" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A7" s="55"/>
-      <c r="B7" s="48" t="s">
+      <c r="A7" s="67"/>
+      <c r="B7" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="50"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="12">
         <v>15</v>
       </c>
@@ -1069,17 +1076,17 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A8" s="55"/>
-      <c r="B8" s="51" t="s">
+      <c r="A8" s="67"/>
+      <c r="B8" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="53"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="39"/>
       <c r="J8" s="5">
         <v>12</v>
       </c>
@@ -1088,17 +1095,17 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A9" s="55"/>
-      <c r="B9" s="16" t="s">
+      <c r="A9" s="67"/>
+      <c r="B9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
       <c r="J9" s="2">
         <v>15</v>
       </c>
@@ -1107,17 +1114,17 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A10" s="55"/>
-      <c r="B10" s="51" t="s">
+      <c r="A10" s="67"/>
+      <c r="B10" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="53"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
       <c r="J10" s="5">
         <v>18</v>
       </c>
@@ -1126,17 +1133,17 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A11" s="55"/>
-      <c r="B11" s="22" t="s">
+      <c r="A11" s="67"/>
+      <c r="B11" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="24"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="51"/>
       <c r="J11" s="12">
         <v>20</v>
       </c>
@@ -1145,17 +1152,17 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A12" s="55"/>
-      <c r="B12" s="35" t="s">
+      <c r="A12" s="67"/>
+      <c r="B12" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="45"/>
       <c r="J12" s="5">
         <v>15</v>
       </c>
@@ -1164,104 +1171,106 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A13" s="56"/>
-      <c r="B13" s="48" t="s">
+      <c r="A13" s="68"/>
+      <c r="B13" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="50"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="11">
         <v>15</v>
       </c>
-      <c r="K13" s="1"/>
+      <c r="K13" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="37"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="45"/>
       <c r="J14" s="2">
         <v>15</v>
       </c>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A15" s="34"/>
-      <c r="B15" s="51" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="53"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="2">
         <v>10</v>
       </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="37"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
       <c r="J16" s="2">
         <v>15</v>
       </c>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A17" s="34"/>
-      <c r="B17" s="19" t="s">
+      <c r="A17" s="17"/>
+      <c r="B17" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="21"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
       <c r="J17" s="11">
         <v>15</v>
       </c>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A18" s="33"/>
-      <c r="B18" s="64" t="s">
+      <c r="A18" s="58"/>
+      <c r="B18" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="66"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="48"/>
       <c r="J18" s="9">
         <v>35</v>
       </c>
@@ -1270,19 +1279,19 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="18"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
       <c r="J19" s="2">
         <v>15</v>
       </c>
@@ -1291,17 +1300,17 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A20" s="34"/>
-      <c r="B20" s="16" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
       <c r="J20" s="2">
         <v>25</v>
       </c>
@@ -1310,17 +1319,17 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A21" s="34"/>
-      <c r="B21" s="61" t="s">
+      <c r="A21" s="17"/>
+      <c r="B21" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="63"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
       <c r="J21" s="2">
         <v>20</v>
       </c>
@@ -1329,17 +1338,17 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A22" s="34"/>
-      <c r="B22" s="61" t="s">
+      <c r="A22" s="17"/>
+      <c r="B22" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="63"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="23"/>
       <c r="J22" s="2">
         <v>20</v>
       </c>
@@ -1348,17 +1357,17 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A23" s="34"/>
-      <c r="B23" s="61" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="63"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="23"/>
       <c r="J23" s="2">
         <v>25</v>
       </c>
@@ -1367,17 +1376,17 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A24" s="33"/>
-      <c r="B24" s="58" t="s">
+      <c r="A24" s="58"/>
+      <c r="B24" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="60"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="36"/>
       <c r="J24" s="9">
         <v>15</v>
       </c>
@@ -1386,19 +1395,19 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="63"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="23"/>
       <c r="J25" s="2">
         <v>15</v>
       </c>
@@ -1407,51 +1416,55 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A26" s="34"/>
-      <c r="B26" s="61" t="s">
+      <c r="A26" s="17"/>
+      <c r="B26" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="63"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="23"/>
       <c r="J26" s="2">
         <v>15</v>
       </c>
-      <c r="K26" s="1"/>
+      <c r="K26" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A27" s="34"/>
-      <c r="B27" s="61" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="63"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="23"/>
       <c r="J27" s="2">
         <v>25</v>
       </c>
-      <c r="K27" s="1"/>
+      <c r="K27" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A28" s="34"/>
-      <c r="B28" s="58" t="s">
+      <c r="A28" s="17"/>
+      <c r="B28" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="60"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="36"/>
       <c r="J28" s="9">
         <v>15</v>
       </c>
@@ -1460,17 +1473,17 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A29" s="34"/>
-      <c r="B29" s="58" t="s">
+      <c r="A29" s="17"/>
+      <c r="B29" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="60"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="36"/>
       <c r="J29" s="9">
         <v>25</v>
       </c>
@@ -1479,19 +1492,19 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A30" s="67" t="s">
+      <c r="A30" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="70" t="s">
+      <c r="B30" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="72"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="26"/>
       <c r="J30" s="6">
         <v>12</v>
       </c>
@@ -1500,17 +1513,17 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A31" s="68"/>
-      <c r="B31" s="73" t="s">
+      <c r="A31" s="19"/>
+      <c r="B31" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="74"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="74"/>
-      <c r="I31" s="75"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="29"/>
       <c r="J31" s="7">
         <v>12</v>
       </c>
@@ -1519,51 +1532,55 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A32" s="68"/>
-      <c r="B32" s="73" t="s">
+      <c r="A32" s="19"/>
+      <c r="B32" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="74"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="75"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="29"/>
       <c r="J32" s="7">
         <v>12</v>
       </c>
-      <c r="K32" s="1"/>
+      <c r="K32" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="33" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A33" s="68"/>
-      <c r="B33" s="73" t="s">
+      <c r="A33" s="19"/>
+      <c r="B33" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="74"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="75"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="29"/>
       <c r="J33" s="6">
         <v>12</v>
       </c>
-      <c r="K33" s="1"/>
+      <c r="K33" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="34" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A34" s="68"/>
-      <c r="B34" s="76" t="s">
+      <c r="A34" s="19"/>
+      <c r="B34" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="78"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="32"/>
       <c r="J34" s="6">
         <v>14</v>
       </c>
@@ -1572,17 +1589,17 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A35" s="68"/>
-      <c r="B35" s="16" t="s">
+      <c r="A35" s="19"/>
+      <c r="B35" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="18"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="15"/>
       <c r="J35" s="2">
         <v>15</v>
       </c>
@@ -1591,70 +1608,74 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A36" s="68"/>
-      <c r="B36" s="16" t="s">
+      <c r="A36" s="19"/>
+      <c r="B36" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="18"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="15"/>
       <c r="J36" s="2">
         <v>30</v>
       </c>
-      <c r="K36" s="1"/>
+      <c r="K36" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="37" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A37" s="68"/>
-      <c r="B37" s="16" t="s">
+      <c r="A37" s="19"/>
+      <c r="B37" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="18"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="15"/>
       <c r="J37" s="2">
         <v>15</v>
       </c>
       <c r="K37" s="1"/>
     </row>
     <row r="38" spans="1:11" ht="39.9" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A38" s="69"/>
-      <c r="B38" s="29" t="s">
+      <c r="A38" s="20"/>
+      <c r="B38" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="31"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="77"/>
+      <c r="G38" s="77"/>
+      <c r="H38" s="77"/>
+      <c r="I38" s="78"/>
       <c r="J38" s="2">
         <v>30</v>
       </c>
-      <c r="K38" s="1"/>
+      <c r="K38" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="39" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="18"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="15"/>
       <c r="J39" s="2">
         <v>10</v>
       </c>
@@ -1663,17 +1684,17 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A40" s="34"/>
-      <c r="B40" s="19" t="s">
+      <c r="A40" s="17"/>
+      <c r="B40" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="21"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="54"/>
       <c r="J40" s="11">
         <v>30</v>
       </c>
@@ -1682,17 +1703,17 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A41" s="34"/>
-      <c r="B41" s="19" t="s">
+      <c r="A41" s="17"/>
+      <c r="B41" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="21"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="54"/>
       <c r="J41" s="11">
         <v>35</v>
       </c>
@@ -1701,17 +1722,17 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A42" s="34"/>
-      <c r="B42" s="22" t="s">
+      <c r="A42" s="17"/>
+      <c r="B42" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="24"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="51"/>
       <c r="J42" s="12">
         <v>20</v>
       </c>
@@ -1720,17 +1741,17 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="33"/>
-      <c r="B43" s="25" t="s">
+      <c r="A43" s="58"/>
+      <c r="B43" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="27"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="73"/>
+      <c r="I43" s="74"/>
       <c r="J43" s="10">
         <v>50</v>
       </c>
@@ -1739,19 +1760,19 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="28" t="s">
+      <c r="B44" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="28"/>
+      <c r="C44" s="75"/>
+      <c r="D44" s="75"/>
+      <c r="E44" s="75"/>
+      <c r="F44" s="75"/>
+      <c r="G44" s="75"/>
+      <c r="H44" s="75"/>
+      <c r="I44" s="75"/>
       <c r="J44" s="5">
         <v>15</v>
       </c>
@@ -1760,17 +1781,17 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
-      <c r="B45" s="28" t="s">
+      <c r="A45" s="58"/>
+      <c r="B45" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
+      <c r="C45" s="75"/>
+      <c r="D45" s="75"/>
+      <c r="E45" s="75"/>
+      <c r="F45" s="75"/>
+      <c r="G45" s="75"/>
+      <c r="H45" s="75"/>
+      <c r="I45" s="75"/>
       <c r="J45" s="5">
         <v>15</v>
       </c>
@@ -1782,12 +1803,12 @@
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="13" t="s">
+      <c r="F46" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="15"/>
+      <c r="G46" s="70"/>
+      <c r="H46" s="70"/>
+      <c r="I46" s="71"/>
       <c r="J46" s="4">
         <f>SUM(J3:J5, J8:J10, J19:J23, J25:J27, J30:J39, J12, J14:J16, J44:J45)</f>
         <v>472</v>
@@ -1795,21 +1816,21 @@
       <c r="K46" s="1"/>
     </row>
     <row r="47" spans="1:11" ht="25.8" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="15"/>
+      <c r="B47" s="70"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="71"/>
       <c r="E47" s="4">
         <v>640</v>
       </c>
-      <c r="F47" s="13" t="s">
+      <c r="F47" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="15"/>
+      <c r="G47" s="70"/>
+      <c r="H47" s="70"/>
+      <c r="I47" s="71"/>
       <c r="J47" s="4">
         <f>SUM(J6:J7, J11, J40:J42, J13, J17)</f>
         <v>168</v>
@@ -1822,12 +1843,12 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="13" t="s">
+      <c r="F48" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="15"/>
+      <c r="G48" s="70"/>
+      <c r="H48" s="70"/>
+      <c r="I48" s="71"/>
       <c r="J48" s="4">
         <f>SUM(J24, J18, J28:J29, J43)</f>
         <v>140</v>
@@ -1840,12 +1861,12 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="13" t="s">
+      <c r="F49" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="15"/>
+      <c r="G49" s="70"/>
+      <c r="H49" s="70"/>
+      <c r="I49" s="71"/>
       <c r="J49" s="4">
         <f>SUM(J3:J45)</f>
         <v>780</v>
@@ -1854,17 +1875,36 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="B39:I39"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A30:A38"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B30:I30"/>
-    <mergeCell ref="B31:I31"/>
-    <mergeCell ref="B32:I32"/>
-    <mergeCell ref="B33:I33"/>
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="B45:I45"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="B37:I37"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="B13:I13"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="B28:I28"/>
     <mergeCell ref="B29:I29"/>
@@ -1881,36 +1921,17 @@
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B12:I12"/>
     <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="A5:A13"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B40:I40"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="B43:I43"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="B45:I45"/>
-    <mergeCell ref="B41:I41"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="B37:I37"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B39:I39"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="B36:I36"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Subcircuit features finally completed!
</commit_message>
<xml_diff>
--- a/OOP2025_Project_ScoresAllocation (2).xlsx
+++ b/OOP2025_Project_ScoresAllocation (2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erfan\Dev\Cpp\sutSpice_phase2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3877D6AB-D793-48D8-B3A8-FF0E46E55F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3F898D-60BC-4B03-9398-68C2EC0F50EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="60">
   <si>
     <t>عنوان</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>تحلیل Phase Sweep (در حضور صرفا یک منبع ولتاژ Phase)</t>
+  </si>
+  <si>
+    <t>ذخیره و استفاده از تک قطبی ها بصورت مدار معادل تونن یا نورتون(مدار مقاومتی)</t>
   </si>
 </sst>
 </file>
@@ -520,6 +523,177 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -527,33 +701,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="6" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -576,150 +723,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="7" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -948,8 +951,8 @@
   </sheetPr>
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A35" zoomScale="118" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A8" zoomScale="74" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -960,49 +963,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="40"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="58"/>
       <c r="J2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="42"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="61"/>
       <c r="J3" s="2">
         <v>5</v>
       </c>
@@ -1011,34 +1014,34 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="63"/>
       <c r="J4" s="2"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="66"/>
       <c r="J5" s="2">
         <v>15</v>
       </c>
@@ -1047,17 +1050,17 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A6" s="55"/>
-      <c r="B6" s="48" t="s">
+      <c r="A6" s="68"/>
+      <c r="B6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="50"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="42"/>
       <c r="J6" s="11">
         <v>18</v>
       </c>
@@ -1066,17 +1069,17 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A7" s="55"/>
-      <c r="B7" s="48" t="s">
+      <c r="A7" s="68"/>
+      <c r="B7" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="50"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="12">
         <v>15</v>
       </c>
@@ -1085,17 +1088,17 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A8" s="55"/>
-      <c r="B8" s="51" t="s">
+      <c r="A8" s="68"/>
+      <c r="B8" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="53"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="39"/>
       <c r="J8" s="5">
         <v>12</v>
       </c>
@@ -1104,17 +1107,17 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A9" s="55"/>
-      <c r="B9" s="16" t="s">
+      <c r="A9" s="68"/>
+      <c r="B9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
       <c r="J9" s="2">
         <v>15</v>
       </c>
@@ -1123,17 +1126,17 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A10" s="55"/>
-      <c r="B10" s="51" t="s">
+      <c r="A10" s="68"/>
+      <c r="B10" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="53"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
       <c r="J10" s="5">
         <v>18</v>
       </c>
@@ -1142,17 +1145,17 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A11" s="55"/>
-      <c r="B11" s="22" t="s">
+      <c r="A11" s="68"/>
+      <c r="B11" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="24"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="51"/>
       <c r="J11" s="12">
         <v>20</v>
       </c>
@@ -1161,17 +1164,17 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A12" s="55"/>
-      <c r="B12" s="35" t="s">
+      <c r="A12" s="68"/>
+      <c r="B12" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="45"/>
       <c r="J12" s="5">
         <v>15</v>
       </c>
@@ -1180,17 +1183,17 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A13" s="56"/>
-      <c r="B13" s="48" t="s">
+      <c r="A13" s="69"/>
+      <c r="B13" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="50"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="11">
         <v>15</v>
       </c>
@@ -1199,108 +1202,116 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="37"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="45"/>
       <c r="J14" s="2">
         <v>15</v>
       </c>
-      <c r="K14" s="1"/>
+      <c r="K14" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A15" s="34"/>
-      <c r="B15" s="51" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="53"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="2">
         <v>10</v>
       </c>
-      <c r="K15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="37"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
       <c r="J16" s="2">
         <v>15</v>
       </c>
-      <c r="K16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A17" s="34"/>
-      <c r="B17" s="19" t="s">
+      <c r="A17" s="17"/>
+      <c r="B17" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="21"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="55"/>
       <c r="J17" s="11">
         <v>15</v>
       </c>
-      <c r="K17" s="1"/>
+      <c r="K17" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A18" s="33"/>
-      <c r="B18" s="64" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="66"/>
+      <c r="A18" s="59"/>
+      <c r="B18" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="48"/>
       <c r="J18" s="9">
         <v>35</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="18"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
       <c r="J19" s="2">
         <v>15</v>
       </c>
@@ -1309,17 +1320,17 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A20" s="34"/>
-      <c r="B20" s="16" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
       <c r="J20" s="2">
         <v>25</v>
       </c>
@@ -1328,17 +1339,17 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A21" s="34"/>
-      <c r="B21" s="61" t="s">
+      <c r="A21" s="17"/>
+      <c r="B21" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="63"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
       <c r="J21" s="2">
         <v>20</v>
       </c>
@@ -1347,17 +1358,17 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A22" s="34"/>
-      <c r="B22" s="61" t="s">
+      <c r="A22" s="17"/>
+      <c r="B22" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="63"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="23"/>
       <c r="J22" s="2">
         <v>20</v>
       </c>
@@ -1366,17 +1377,17 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A23" s="34"/>
-      <c r="B23" s="61" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="63"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="23"/>
       <c r="J23" s="2">
         <v>25</v>
       </c>
@@ -1385,17 +1396,17 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A24" s="33"/>
-      <c r="B24" s="58" t="s">
+      <c r="A24" s="59"/>
+      <c r="B24" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="60"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="36"/>
       <c r="J24" s="9">
         <v>15</v>
       </c>
@@ -1404,19 +1415,19 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="63"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="23"/>
       <c r="J25" s="2">
         <v>15</v>
       </c>
@@ -1425,17 +1436,17 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A26" s="34"/>
-      <c r="B26" s="61" t="s">
+      <c r="A26" s="17"/>
+      <c r="B26" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="63"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="23"/>
       <c r="J26" s="2">
         <v>15</v>
       </c>
@@ -1444,17 +1455,17 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A27" s="34"/>
-      <c r="B27" s="61" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="63"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="23"/>
       <c r="J27" s="2">
         <v>25</v>
       </c>
@@ -1463,17 +1474,17 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A28" s="34"/>
-      <c r="B28" s="79" t="s">
+      <c r="A28" s="17"/>
+      <c r="B28" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="60"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="36"/>
       <c r="J28" s="9">
         <v>15</v>
       </c>
@@ -1482,17 +1493,17 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A29" s="34"/>
-      <c r="B29" s="79" t="s">
+      <c r="A29" s="17"/>
+      <c r="B29" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="60"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="36"/>
       <c r="J29" s="9">
         <v>25</v>
       </c>
@@ -1501,19 +1512,19 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A30" s="67" t="s">
+      <c r="A30" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="70" t="s">
+      <c r="B30" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="72"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="26"/>
       <c r="J30" s="6">
         <v>12</v>
       </c>
@@ -1522,17 +1533,17 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A31" s="68"/>
-      <c r="B31" s="73" t="s">
+      <c r="A31" s="19"/>
+      <c r="B31" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="74"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="74"/>
-      <c r="I31" s="75"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="29"/>
       <c r="J31" s="7">
         <v>12</v>
       </c>
@@ -1541,17 +1552,17 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A32" s="68"/>
-      <c r="B32" s="73" t="s">
+      <c r="A32" s="19"/>
+      <c r="B32" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="74"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="75"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="29"/>
       <c r="J32" s="7">
         <v>12</v>
       </c>
@@ -1560,17 +1571,17 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A33" s="68"/>
-      <c r="B33" s="73" t="s">
+      <c r="A33" s="19"/>
+      <c r="B33" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="74"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="75"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="29"/>
       <c r="J33" s="6">
         <v>12</v>
       </c>
@@ -1579,17 +1590,17 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A34" s="68"/>
-      <c r="B34" s="76" t="s">
+      <c r="A34" s="19"/>
+      <c r="B34" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="78"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="32"/>
       <c r="J34" s="6">
         <v>14</v>
       </c>
@@ -1598,17 +1609,17 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A35" s="68"/>
-      <c r="B35" s="16" t="s">
+      <c r="A35" s="19"/>
+      <c r="B35" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="18"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="15"/>
       <c r="J35" s="2">
         <v>15</v>
       </c>
@@ -1617,17 +1628,17 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A36" s="68"/>
-      <c r="B36" s="16" t="s">
+      <c r="A36" s="19"/>
+      <c r="B36" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="18"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="15"/>
       <c r="J36" s="2">
         <v>30</v>
       </c>
@@ -1636,34 +1647,36 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A37" s="68"/>
-      <c r="B37" s="16" t="s">
+      <c r="A37" s="19"/>
+      <c r="B37" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="18"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="15"/>
       <c r="J37" s="2">
         <v>15</v>
       </c>
-      <c r="K37" s="1"/>
+      <c r="K37" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="38" spans="1:11" ht="39.9" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A38" s="69"/>
-      <c r="B38" s="29" t="s">
+      <c r="A38" s="20"/>
+      <c r="B38" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="31"/>
+      <c r="C38" s="78"/>
+      <c r="D38" s="78"/>
+      <c r="E38" s="78"/>
+      <c r="F38" s="78"/>
+      <c r="G38" s="78"/>
+      <c r="H38" s="78"/>
+      <c r="I38" s="79"/>
       <c r="J38" s="2">
         <v>30</v>
       </c>
@@ -1672,19 +1685,19 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="18"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="15"/>
       <c r="J39" s="2">
         <v>10</v>
       </c>
@@ -1693,17 +1706,17 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A40" s="34"/>
-      <c r="B40" s="19" t="s">
+      <c r="A40" s="17"/>
+      <c r="B40" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="21"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54"/>
+      <c r="I40" s="55"/>
       <c r="J40" s="11">
         <v>30</v>
       </c>
@@ -1712,17 +1725,17 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A41" s="34"/>
-      <c r="B41" s="19" t="s">
+      <c r="A41" s="17"/>
+      <c r="B41" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="21"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
+      <c r="I41" s="55"/>
       <c r="J41" s="11">
         <v>35</v>
       </c>
@@ -1731,17 +1744,17 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A42" s="34"/>
-      <c r="B42" s="22" t="s">
+      <c r="A42" s="17"/>
+      <c r="B42" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="24"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="51"/>
       <c r="J42" s="12">
         <v>20</v>
       </c>
@@ -1750,17 +1763,17 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="33"/>
-      <c r="B43" s="25" t="s">
+      <c r="A43" s="59"/>
+      <c r="B43" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="27"/>
+      <c r="C43" s="74"/>
+      <c r="D43" s="74"/>
+      <c r="E43" s="74"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="75"/>
       <c r="J43" s="10">
         <v>50</v>
       </c>
@@ -1769,19 +1782,19 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="28" t="s">
+      <c r="B44" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="28"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="76"/>
+      <c r="G44" s="76"/>
+      <c r="H44" s="76"/>
+      <c r="I44" s="76"/>
       <c r="J44" s="5">
         <v>15</v>
       </c>
@@ -1790,17 +1803,17 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
-      <c r="B45" s="28" t="s">
+      <c r="A45" s="59"/>
+      <c r="B45" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
+      <c r="C45" s="76"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="76"/>
+      <c r="F45" s="76"/>
+      <c r="G45" s="76"/>
+      <c r="H45" s="76"/>
+      <c r="I45" s="76"/>
       <c r="J45" s="5">
         <v>15</v>
       </c>
@@ -1812,12 +1825,12 @@
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="13" t="s">
+      <c r="F46" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="15"/>
+      <c r="G46" s="71"/>
+      <c r="H46" s="71"/>
+      <c r="I46" s="72"/>
       <c r="J46" s="4">
         <f>SUM(J3:J5, J8:J10, J19:J23, J25:J27, J30:J39, J12, J14:J16, J44:J45)</f>
         <v>472</v>
@@ -1825,21 +1838,21 @@
       <c r="K46" s="1"/>
     </row>
     <row r="47" spans="1:11" ht="25.8" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="15"/>
+      <c r="B47" s="71"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="72"/>
       <c r="E47" s="4">
         <v>640</v>
       </c>
-      <c r="F47" s="13" t="s">
+      <c r="F47" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="15"/>
+      <c r="G47" s="71"/>
+      <c r="H47" s="71"/>
+      <c r="I47" s="72"/>
       <c r="J47" s="4">
         <f>SUM(J6:J7, J11, J40:J42, J13, J17)</f>
         <v>168</v>
@@ -1852,12 +1865,12 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="13" t="s">
+      <c r="F48" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="15"/>
+      <c r="G48" s="71"/>
+      <c r="H48" s="71"/>
+      <c r="I48" s="72"/>
       <c r="J48" s="4">
         <f>SUM(J24, J18, J28:J29, J43)</f>
         <v>140</v>
@@ -1870,12 +1883,12 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="13" t="s">
+      <c r="F49" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="15"/>
+      <c r="G49" s="71"/>
+      <c r="H49" s="71"/>
+      <c r="I49" s="72"/>
       <c r="J49" s="4">
         <f>SUM(J3:J45)</f>
         <v>780</v>
@@ -1884,17 +1897,36 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="B39:I39"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A30:A38"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B30:I30"/>
-    <mergeCell ref="B31:I31"/>
-    <mergeCell ref="B32:I32"/>
-    <mergeCell ref="B33:I33"/>
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="B43:I43"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="B45:I45"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="B37:I37"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="B13:I13"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="B28:I28"/>
     <mergeCell ref="B29:I29"/>
@@ -1911,36 +1943,17 @@
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B12:I12"/>
     <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="A5:A13"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B40:I40"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="B43:I43"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="B45:I45"/>
-    <mergeCell ref="B41:I41"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="B37:I37"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B39:I39"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="B36:I36"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>